<commit_message>
Atualizando a tabela Q2_A
</commit_message>
<xml_diff>
--- a/tabelas_para_relatório.xlsx
+++ b/tabelas_para_relatório.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Função</t>
   </si>
@@ -74,9 +74,6 @@
     <t>SLL</t>
   </si>
   <si>
-    <t>O resultado é o iB deslocado iShamt vezes para a esquerda</t>
-  </si>
-  <si>
     <t>00100</t>
   </si>
   <si>
@@ -99,14 +96,148 @@
   </si>
   <si>
     <t>SLT</t>
+  </si>
+  <si>
+    <t>00111</t>
+  </si>
+  <si>
+    <t>Retorna 1 se iA for menor que iB, retorna 0 caso contrario</t>
+  </si>
+  <si>
+    <t>SRL</t>
+  </si>
+  <si>
+    <t>01000</t>
+  </si>
+  <si>
+    <t>SRA</t>
+  </si>
+  <si>
+    <t>01001</t>
+  </si>
+  <si>
+    <t>O resultado é o iB deslocado iShamt vezes para a direita, completando os bit mais siguinificativos com zero</t>
+  </si>
+  <si>
+    <t>O resultado é o iB deslocado iShamt vezes para a esquerda, completando os bits menos siguinificativos com zeros</t>
+  </si>
+  <si>
+    <t>O resultado é o iB deslocado iShamt vezes para a direita, completando os bit mais siguinificativos com o memos nível lógico do bit mais siguinificativo</t>
+  </si>
+  <si>
+    <t>XOR</t>
+  </si>
+  <si>
+    <t>01010</t>
+  </si>
+  <si>
+    <t>O resultado é iqual a um XOR bit a bit do iA com o iB</t>
+  </si>
+  <si>
+    <t>SLTU</t>
+  </si>
+  <si>
+    <t>01011</t>
+  </si>
+  <si>
+    <t>Retorna 1 se iA for menor que iB considerando representação sem sinal, retorna 0 caso contrario</t>
+  </si>
+  <si>
+    <t>NOR</t>
+  </si>
+  <si>
+    <t>O resultado é iqual a um NOR bit a bit do iA com o iB</t>
+  </si>
+  <si>
+    <t>01100</t>
+  </si>
+  <si>
+    <t>MULT</t>
+  </si>
+  <si>
+    <t>01110</t>
+  </si>
+  <si>
+    <t>01101</t>
+  </si>
+  <si>
+    <t>01111</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>10010</t>
+  </si>
+  <si>
+    <t>10011</t>
+  </si>
+  <si>
+    <t>10100</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>LUI</t>
+  </si>
+  <si>
+    <t>SLLV</t>
+  </si>
+  <si>
+    <t>SRAV</t>
+  </si>
+  <si>
+    <t>SRLV</t>
+  </si>
+  <si>
+    <t>MULTU</t>
+  </si>
+  <si>
+    <t>DIVU</t>
+  </si>
+  <si>
+    <t>O HI recebe os 32bits mais siguinificativos da multiplicação de Ai por Bi e LO recebe os os 32 menso siginificativos dessa multiplicação. E o resultado recebe o valor de LO</t>
+  </si>
+  <si>
+    <t>O HI recebe resultado da divisão de Ai por Bi e LO recebe o resto dessa sivisão. E o resultado recebe o valor de LO</t>
+  </si>
+  <si>
+    <t>Os 16bits mais siguinificativos do resultado recebem ao valor de iB e os 16 bits menos siguinificativos recebem zeros</t>
+  </si>
+  <si>
+    <t>O resultado é o iB deslocado para a direita o número guardado nos 5 bits menos siguinificativos de iA, completando os bits mais siguinificativos do resultado com zeros com o mesmo valor lógico do bit mais siguinificativo de Bi</t>
+  </si>
+  <si>
+    <t>O resultado é o iB deslocado para a esquerda o numero guardado nos 5 bits menos siguinificativos de iA, completando os bits menos siguinificativos do rtesultado com zeros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O resultado é o iB deslocado para a direita o número guardado nos 5 bits menos siguinificativos de iA, completando os bits menos siguinificativos  com o mesmo valor lógico do bit mais significativo do rtesultado </t>
+  </si>
+  <si>
+    <t>O HI recebe os 32bits mais siguinificativos da multiplicação sem sinal de Ai por Bi e LO recebe os os 32 menso siginificativos dessa multiplicação. E o resultado recebe o valor de LO</t>
+  </si>
+  <si>
+    <t>O HI recebe resultado da divisão sem sinal de Ai por Bi e LO recebe o resto dessa sivisão. E o resultado recebe o valor de LO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -139,10 +270,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -177,8 +308,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C22" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C22"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Função" dataDxfId="3"/>
     <tableColumn id="2" name="Descrição" dataDxfId="2"/>
@@ -451,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +613,7 @@
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -493,7 +624,7 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -504,7 +635,7 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -515,53 +646,205 @@
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>